<commit_message>
lets do a retry
</commit_message>
<xml_diff>
--- a/Cleaned Data XLS format/Illinois_Mean_Salary.xlsx
+++ b/Cleaned Data XLS format/Illinois_Mean_Salary.xlsx
@@ -1,34 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boston\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quentinsloboda/OnTheUpAndUp/Cleaned Data XLS format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE3B3E0-4EA1-426D-A2BC-6943015DE16D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F9B919-78EB-F049-B05A-E82961FC78D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="675" windowWidth="21810" windowHeight="11865" xr2:uid="{A3F38FD2-2162-416F-9FD3-CAC97CBAFA4D}"/>
+    <workbookView xWindow="-35440" yWindow="340" windowWidth="21820" windowHeight="11860" xr2:uid="{A3F38FD2-2162-416F-9FD3-CAC97CBAFA4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
-  <si>
-    <t>https://www.bls.gov/oes/tables.htm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Median Hourly Wage</t>
   </si>
@@ -106,9 +112,6 @@
   </si>
   <si>
     <t>Median Weekly Earnings</t>
-  </si>
-  <si>
-    <t>Occupation: Computer and information systems managers</t>
   </si>
   <si>
     <t>Annual Median Wage</t>
@@ -123,7 +126,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,14 +266,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -570,7 +565,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -614,9 +609,8 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -630,7 +624,6 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -716,18 +709,11 @@
     <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="17" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="20" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="23" builtinId="38" customBuiltin="1"/>
@@ -761,7 +747,6 @@
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="3" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="4" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
     <cellStyle name="Input" xfId="7" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="10" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral 2" xfId="40" xr:uid="{3A4514CE-1D6E-43E6-94C7-7B7C1C7C541B}"/>
@@ -1083,589 +1068,564 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BEFB26-5FD5-4F15-AABE-B89102013008}">
-  <dimension ref="A1:V27"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="N3" s="5"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="C4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="34" t="s">
+      <c r="E1" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C5" s="6">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
         <v>2019</v>
       </c>
-      <c r="D5" s="9">
+      <c r="B2" s="8">
         <v>43.32</v>
       </c>
-      <c r="E5" s="10">
+      <c r="C2" s="9">
         <v>90110</v>
       </c>
-      <c r="F5" s="9">
+      <c r="D2" s="8">
         <v>41.89</v>
       </c>
-      <c r="G5" s="10">
-        <f>40*F5</f>
+      <c r="E2" s="9">
+        <f>40*D2</f>
         <v>1675.6</v>
       </c>
-      <c r="H5" s="10">
-        <f>G5*50</f>
+      <c r="F2" s="9">
+        <f>E2*50</f>
         <v>83780</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C6" s="7">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
         <v>2018</v>
       </c>
-      <c r="D6" s="9">
+      <c r="B3" s="8">
         <v>42.17</v>
       </c>
-      <c r="E6" s="10">
+      <c r="C3" s="9">
         <v>87720</v>
       </c>
-      <c r="F6" s="9">
+      <c r="D3" s="8">
         <v>40.65</v>
       </c>
-      <c r="G6" s="10">
-        <f t="shared" ref="G6:G21" si="0">40*F6</f>
+      <c r="E3" s="9">
+        <f t="shared" ref="E3:E18" si="0">40*D3</f>
         <v>1626</v>
       </c>
-      <c r="H6" s="10">
-        <f t="shared" ref="H6:H21" si="1">G6*50</f>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:F18" si="1">E3*50</f>
         <v>81300</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C7" s="7">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
         <v>2017</v>
       </c>
-      <c r="D7" s="9">
+      <c r="B4" s="8">
         <v>41.74</v>
       </c>
-      <c r="E7" s="10">
+      <c r="C4" s="9">
         <v>86820</v>
       </c>
-      <c r="F7" s="9">
+      <c r="D4" s="8">
         <v>40.130000000000003</v>
       </c>
-      <c r="G7" s="10">
+      <c r="E4" s="9">
         <f t="shared" si="0"/>
         <v>1605.2</v>
       </c>
-      <c r="H7" s="10">
+      <c r="F4" s="9">
         <f t="shared" si="1"/>
         <v>80260</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="7">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
         <v>2016</v>
       </c>
-      <c r="D8" s="9">
+      <c r="B5" s="8">
         <v>41.03</v>
       </c>
-      <c r="E8" s="10">
+      <c r="C5" s="9">
         <v>85340</v>
       </c>
-      <c r="F8" s="9">
+      <c r="D5" s="8">
         <v>39.58</v>
       </c>
-      <c r="G8" s="10">
+      <c r="E5" s="9">
         <f t="shared" si="0"/>
         <v>1583.1999999999998</v>
       </c>
-      <c r="H8" s="10">
+      <c r="F5" s="9">
         <f t="shared" si="1"/>
         <v>79159.999999999985</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C9" s="7">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
         <v>2015</v>
       </c>
-      <c r="D9" s="31">
+      <c r="B6" s="30">
         <v>39.68</v>
       </c>
-      <c r="E9" s="33">
+      <c r="C6" s="32">
         <v>82540</v>
       </c>
-      <c r="F9" s="31">
+      <c r="D6" s="30">
         <v>38.54</v>
       </c>
-      <c r="G9" s="10">
+      <c r="E6" s="9">
         <f t="shared" si="0"/>
         <v>1541.6</v>
       </c>
-      <c r="H9" s="10">
+      <c r="F6" s="9">
         <f t="shared" si="1"/>
         <v>77080</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C10" s="7">
+      <c r="G6" s="14"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
         <v>2014</v>
       </c>
-      <c r="D10" s="31">
+      <c r="B7" s="30">
         <v>38.299999999999997</v>
       </c>
-      <c r="E10" s="33">
+      <c r="C7" s="32">
         <v>79670</v>
       </c>
-      <c r="F10" s="31">
+      <c r="D7" s="30">
         <v>37.43</v>
       </c>
-      <c r="G10" s="10">
+      <c r="E7" s="9">
         <f t="shared" si="0"/>
         <v>1497.2</v>
       </c>
-      <c r="H10" s="10">
+      <c r="F7" s="9">
         <f t="shared" si="1"/>
         <v>74860</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C11" s="7">
+      <c r="G7" s="17"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
         <v>2013</v>
       </c>
-      <c r="D11" s="31">
+      <c r="B8" s="30">
         <v>37.630000000000003</v>
       </c>
-      <c r="E11" s="33">
+      <c r="C8" s="32">
         <v>78260</v>
       </c>
-      <c r="F11" s="31">
+      <c r="D8" s="30">
         <v>36.86</v>
       </c>
-      <c r="G11" s="10">
+      <c r="E8" s="9">
         <f t="shared" si="0"/>
         <v>1474.4</v>
       </c>
-      <c r="H11" s="10">
+      <c r="F8" s="9">
         <f t="shared" si="1"/>
         <v>73720</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C12" s="7">
+      <c r="G8" s="20"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
         <v>2012</v>
       </c>
-      <c r="D12" s="31">
+      <c r="B9" s="30">
         <v>37.26</v>
       </c>
-      <c r="E12" s="33">
+      <c r="C9" s="32">
         <v>77500</v>
       </c>
-      <c r="F12" s="31">
+      <c r="D9" s="30">
         <v>36.26</v>
       </c>
-      <c r="G12" s="10">
+      <c r="E9" s="9">
         <f t="shared" si="0"/>
         <v>1450.3999999999999</v>
       </c>
-      <c r="H12" s="10">
+      <c r="F9" s="9">
         <f t="shared" si="1"/>
         <v>72520</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C13" s="7">
+      <c r="G9" s="23"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
         <v>2011</v>
       </c>
-      <c r="D13" s="31">
+      <c r="B10" s="30">
         <v>36.630000000000003</v>
       </c>
-      <c r="E13" s="33">
+      <c r="C10" s="32">
         <v>76180</v>
       </c>
-      <c r="F13" s="31">
+      <c r="D10" s="30">
         <v>35.29</v>
       </c>
-      <c r="G13" s="10">
+      <c r="E10" s="9">
         <f t="shared" si="0"/>
         <v>1411.6</v>
       </c>
-      <c r="H13" s="10">
+      <c r="F10" s="9">
         <f t="shared" si="1"/>
         <v>70580</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C14" s="7">
+      <c r="G10" s="26"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
         <v>2010</v>
       </c>
-      <c r="D14" s="31">
+      <c r="B11" s="30">
         <v>36.119999999999997</v>
       </c>
-      <c r="E14" s="33">
+      <c r="C11" s="32">
         <v>75130</v>
       </c>
-      <c r="F14" s="31">
+      <c r="D11" s="30">
         <v>34.61</v>
       </c>
-      <c r="G14" s="10">
+      <c r="E11" s="9">
         <f t="shared" si="0"/>
         <v>1384.4</v>
       </c>
-      <c r="H14" s="10">
+      <c r="F11" s="9">
         <f t="shared" si="1"/>
         <v>69220</v>
       </c>
-      <c r="I14" s="30"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C15" s="7">
+      <c r="G11" s="29"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>2009</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="B12" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="10">
+      <c r="E12" s="9">
         <f t="shared" si="0"/>
         <v>1392</v>
       </c>
-      <c r="H15" s="10">
+      <c r="F12" s="9">
         <f t="shared" si="1"/>
         <v>69600</v>
       </c>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="33"/>
-      <c r="S15" s="33"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C16" s="7">
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
         <v>2008</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="B13" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="D13" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="10">
+      <c r="E13" s="9">
         <f t="shared" si="0"/>
         <v>1384.8</v>
       </c>
-      <c r="H16" s="10">
+      <c r="F13" s="9">
         <f t="shared" si="1"/>
         <v>69240</v>
       </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C17" s="7">
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>2007</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="B14" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="D14" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="10">
+      <c r="E14" s="9">
         <f t="shared" si="0"/>
         <v>1362.8</v>
       </c>
-      <c r="H17" s="10">
+      <c r="F14" s="9">
         <f t="shared" si="1"/>
         <v>68140</v>
       </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C18" s="7">
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
         <v>2006</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="B15" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="D15" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="10">
+      <c r="E15" s="9">
         <f t="shared" si="0"/>
         <v>1282.4000000000001</v>
       </c>
-      <c r="H18" s="10">
+      <c r="F15" s="9">
         <f t="shared" si="1"/>
         <v>64120.000000000007</v>
       </c>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C19" s="7">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
         <v>2005</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="B16" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="D16" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="10">
+      <c r="E16" s="9">
         <f t="shared" si="0"/>
         <v>1232</v>
       </c>
-      <c r="H19" s="10">
+      <c r="F16" s="9">
         <f t="shared" si="1"/>
         <v>61600</v>
       </c>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C20" s="7">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
         <v>2004</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="B17" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="D17" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="10">
+      <c r="E17" s="9">
         <f t="shared" si="0"/>
         <v>1234.4000000000001</v>
       </c>
-      <c r="H20" s="10">
+      <c r="F17" s="9">
         <f t="shared" si="1"/>
         <v>61720.000000000007</v>
       </c>
     </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C21" s="7">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
         <v>2003</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="B18" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="D18" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="10">
+      <c r="E18" s="9">
         <f t="shared" si="0"/>
         <v>1166</v>
       </c>
-      <c r="H21" s="10">
+      <c r="F18" s="9">
         <f t="shared" si="1"/>
         <v>58300</v>
       </c>
     </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C24" s="7"/>
-    </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C26" s="7"/>
-    </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C27" s="7"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{E23EA04E-11B8-437F-A252-AFFAAE7C4C2B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>